<commit_message>
ultima actualizacion solo de los excel
</commit_message>
<xml_diff>
--- a/9.0 CRONOGRAMA/CRONOGRAMA- CURPAHUASI - 01.xlsx
+++ b/9.0 CRONOGRAMA/CRONOGRAMA- CURPAHUASI - 01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FINANCIERO" sheetId="1" r:id="rId1"/>
@@ -1267,15 +1267,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>55880</xdr:colOff>
+      <xdr:colOff>31664</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>55880</xdr:rowOff>
+      <xdr:rowOff>47808</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>172720</xdr:colOff>
+      <xdr:colOff>148504</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>93528</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1290,8 +1290,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2413000" y="2865120"/>
-          <a:ext cx="1681480" cy="45720"/>
+          <a:off x="2324122" y="2800372"/>
+          <a:ext cx="1642454" cy="45720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1775,8 +1775,8 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1958,10 +1958,12 @@
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="16">
-        <v>9668.3549999999996</v>
+        <f>F12/2</f>
+        <v>31508.89</v>
       </c>
       <c r="D12" s="16">
-        <v>9668.3549999999996</v>
+        <f>F12/2</f>
+        <v>31508.89</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="18">
@@ -2044,11 +2046,11 @@
       </c>
       <c r="C17" s="20">
         <f>SUM(C11:C16)</f>
-        <v>221931.25</v>
+        <v>243771.785</v>
       </c>
       <c r="D17" s="20">
         <f>SUM(D11:D16)</f>
-        <v>96091.079999999987</v>
+        <v>117931.61499999999</v>
       </c>
       <c r="E17" s="20">
         <f>SUM(E11:E16)</f>
@@ -2065,8 +2067,8 @@
       <c r="D18" s="43"/>
       <c r="E18" s="44"/>
       <c r="F18" s="21">
-        <f>SUM(F11:F16)+0.01</f>
-        <v>388994.16</v>
+        <f>SUM(F11:F16)+0</f>
+        <v>388994.14999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2089,8 +2091,8 @@
   </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="118" zoomScaleNormal="110" zoomScaleSheetLayoutView="118" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2585,14 +2587,14 @@
       <c r="E19" s="59"/>
       <c r="F19" s="60">
         <f>FINANCIERO!C17</f>
-        <v>221931.25</v>
+        <v>243771.785</v>
       </c>
       <c r="G19" s="61"/>
       <c r="H19" s="61"/>
       <c r="I19" s="62"/>
       <c r="J19" s="60">
         <f>FINANCIERO!D17</f>
-        <v>96091.079999999987</v>
+        <v>117931.61499999999</v>
       </c>
       <c r="K19" s="61"/>
       <c r="L19" s="61"/>
@@ -2627,8 +2629,8 @@
       <c r="P20" s="53"/>
       <c r="Q20" s="53"/>
       <c r="R20" s="31">
-        <f>SUM(R12:R17)+0.01</f>
-        <v>388994.16</v>
+        <f>SUM(R12:R17)+0</f>
+        <v>388994.14999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>